<commit_message>
updated the chart 02.04-2019
</commit_message>
<xml_diff>
--- a/plan/schedule/gantt-timeline.xlsx
+++ b/plan/schedule/gantt-timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Documents\Studie\Front-End Developing\FED Part Time Course\Semester Project 2019\plan\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20742C4-5E8F-4E9B-AE63-15FCC62CB691}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB2D89A-0626-4A21-BBCD-05C77AE58152}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C7E91EC6-D78D-4019-BD09-36FB01F0F196}"/>
   </bookViews>
@@ -1077,16 +1077,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>137833</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>126628</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>802341</xdr:rowOff>
+      <xdr:rowOff>791135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>147358</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>136153</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>116541</xdr:rowOff>
+      <xdr:rowOff>105335</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1101,7 +1101,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11579039" y="1687606"/>
+          <a:off x="12083304" y="1676400"/>
           <a:ext cx="9525" cy="4973170"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1416,16 +1416,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>257734</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>257734</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1440,8 +1440,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8863852" y="4628029"/>
-          <a:ext cx="1030941" cy="190500"/>
+          <a:off x="8863853" y="4650441"/>
+          <a:ext cx="1266265" cy="179294"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1484,16 +1484,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257734</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>246529</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>246528</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1508,8 +1508,76 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8348382" y="1972235"/>
-          <a:ext cx="762000" cy="179294"/>
+          <a:off x="8348381" y="1972235"/>
+          <a:ext cx="1277471" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>16564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>179293</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rektangel 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CEE2E62-18B4-403C-811F-3A5F99BC4DB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9903077" y="4274799"/>
+          <a:ext cx="507188" cy="162729"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1852,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522C6D6D-DA4F-4D07-9634-46F540085D48}">
   <dimension ref="A1:BP36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new styled header pictures
</commit_message>
<xml_diff>
--- a/plan/schedule/gantt-timeline.xlsx
+++ b/plan/schedule/gantt-timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Documents\Studie\Front-End Developing\FED Part Time Course\Semester Project 2019\plan\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB2D89A-0626-4A21-BBCD-05C77AE58152}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6331E716-01FC-42B4-B8B7-65FC6EFAD891}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C7E91EC6-D78D-4019-BD09-36FB01F0F196}"/>
   </bookViews>
@@ -1077,16 +1077,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>126628</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>146638</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>791135</xdr:rowOff>
+      <xdr:rowOff>763921</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>136153</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>156163</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>105335</xdr:rowOff>
+      <xdr:rowOff>78121</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1101,8 +1101,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12083304" y="1676400"/>
-          <a:ext cx="9525" cy="4973170"/>
+          <a:off x="14447745" y="1661992"/>
+          <a:ext cx="9525" cy="4974772"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1418,12 +1418,12 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>235324</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>244928</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1440,8 +1440,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8863853" y="4650441"/>
-          <a:ext cx="1266265" cy="179294"/>
+          <a:off x="8871857" y="4640036"/>
+          <a:ext cx="1537607" cy="204107"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1490,8 +1490,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>246528</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>231321</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1508,8 +1508,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8348381" y="1972235"/>
-          <a:ext cx="1277471" cy="190500"/>
+          <a:off x="8353984" y="1986643"/>
+          <a:ext cx="2041873" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1578,6 +1578,550 @@
         <a:xfrm>
           <a:off x="9903077" y="4274799"/>
           <a:ext cx="507188" cy="162729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rektangel 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E040216-056B-431C-8A46-4F124F054D05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8354786" y="3891642"/>
+          <a:ext cx="789214" cy="204107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>176894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>244929</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>176894</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rektangel 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C1BBCE-0478-401A-AF77-71C04F1AAE1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9130393" y="4068537"/>
+          <a:ext cx="762000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>244929</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rektangel 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BB54148-44E8-4066-8C6B-CA3BD0210883}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9647464" y="4463143"/>
+          <a:ext cx="503465" cy="163286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>258534</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>258535</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>13606</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Rektangel 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{363F2A88-87DE-4C62-B707-39772C9B1D75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10423070" y="4844142"/>
+          <a:ext cx="1292679" cy="204107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>258535</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>136070</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rektangel 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9279E37B-80A5-4A6D-835F-3E807285ABDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12491356" y="5034643"/>
+          <a:ext cx="653143" cy="204107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>122464</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rektangel 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B939BB2-809A-40DB-A3B1-26791D406C0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14042571" y="5225143"/>
+          <a:ext cx="639536" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>149679</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Rektangel 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20AF23A7-8553-4C9C-BFF4-54097DBDAEFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15593786" y="5415643"/>
+          <a:ext cx="666750" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>27215</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rektangel 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3342E456-B864-4C03-A566-785074B61086}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10450286" y="2177143"/>
+          <a:ext cx="2694214" cy="176893"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1920,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522C6D6D-DA4F-4D07-9634-46F540085D48}">
   <dimension ref="A1:BP36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
first finished launch ready product
</commit_message>
<xml_diff>
--- a/plan/schedule/gantt-timeline.xlsx
+++ b/plan/schedule/gantt-timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Documents\Studie\Front-End Developing\FED Part Time Course\Semester Project 2019\plan\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6331E716-01FC-42B4-B8B7-65FC6EFAD891}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A385D758-4769-48C5-9A07-62BA263558B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C7E91EC6-D78D-4019-BD09-36FB01F0F196}"/>
   </bookViews>
@@ -569,124 +569,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Rett linje 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A39A3995-19C4-451D-B95A-8FAC6B30386E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="990600"/>
-          <a:ext cx="0" cy="2628900"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Rett linje 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A621DA60-6649-4CA1-9DF4-6C947ECC2DA6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10391775" y="1009650"/>
-          <a:ext cx="0" cy="3562350"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="arrow" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>52</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -1077,73 +959,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>146638</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>763921</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>156163</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>78121</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Rett linje 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C147B5DA-E6A9-45C2-AEC9-D56A4B2A82B7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14447745" y="1661992"/>
-          <a:ext cx="9525" cy="4974772"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:headEnd type="triangle" w="med" len="med"/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst>
-          <a:glow rad="228600">
-            <a:schemeClr val="accent6">
-              <a:satMod val="175000"/>
-              <a:alpha val="40000"/>
-            </a:schemeClr>
-          </a:glow>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
@@ -1283,13 +1098,13 @@
       <xdr:col>52</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1304,8 +1119,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18364200" y="6162675"/>
-          <a:ext cx="47625" cy="200025"/>
+          <a:off x="18364200" y="6162676"/>
+          <a:ext cx="180975" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1825,15 +1640,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>258534</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>258532</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>258535</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>13606</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>138545</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1848,8 +1663,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10423070" y="4844142"/>
-          <a:ext cx="1292679" cy="204107"/>
+          <a:off x="10424305" y="4849090"/>
+          <a:ext cx="1958195" cy="173183"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1893,15 +1708,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>258535</xdr:colOff>
+      <xdr:colOff>258534</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>136070</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>121227</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1916,8 +1731,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12491356" y="5034643"/>
-          <a:ext cx="653143" cy="204107"/>
+          <a:off x="12502489" y="5039592"/>
+          <a:ext cx="1421329" cy="190499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1966,10 +1781,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>122464</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>138546</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1984,8 +1799,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14042571" y="5225143"/>
-          <a:ext cx="639536" cy="190500"/>
+          <a:off x="14062364" y="5230091"/>
+          <a:ext cx="1437409" cy="173182"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2028,14 +1843,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>259772</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>138545</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2052,8 +1867,76 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15593786" y="5415643"/>
-          <a:ext cx="666750" cy="190500"/>
+          <a:off x="15620999" y="5420591"/>
+          <a:ext cx="1437410" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>242454</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>103909</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rektangel 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3342E456-B864-4C03-A566-785074B61086}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10408227" y="2182091"/>
+          <a:ext cx="6355773" cy="190499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2097,69 +1980,186 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>27215</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>136071</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="Rektangel 37">
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Rett linje 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3342E456-B864-4C03-A566-785074B61086}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A621DA60-6649-4CA1-9DF4-6C947ECC2DA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10450286" y="2177143"/>
-          <a:ext cx="2694214" cy="176893"/>
+          <a:off x="10391775" y="1009650"/>
+          <a:ext cx="0" cy="3562350"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
+        <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6"/>
-        </a:solidFill>
-        <a:ln>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent6"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx1"/>
         </a:fontRef>
       </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="nb-NO" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Rett linje 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A39A3995-19C4-451D-B95A-8FAC6B30386E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="990600"/>
+          <a:ext cx="0" cy="2628900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>130336</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>775126</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>139861</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>89326</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Rett linje 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C147B5DA-E6A9-45C2-AEC9-D56A4B2A82B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17050200" y="1675671"/>
+          <a:ext cx="9525" cy="4977246"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst>
+          <a:glow rad="228600">
+            <a:schemeClr val="accent6">
+              <a:satMod val="175000"/>
+              <a:alpha val="40000"/>
+            </a:schemeClr>
+          </a:glow>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2465,7 +2465,7 @@
   <dimension ref="A1:BP36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BB12" sqref="BB12"/>
+      <selection activeCell="AR11" sqref="AR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated the gantt chart and document plan, started on report and added templates
</commit_message>
<xml_diff>
--- a/plan/schedule/gantt-timeline.xlsx
+++ b/plan/schedule/gantt-timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Glenn\Documents\Studie\Front-End Developing\FED Part Time Course\Semester Project 2019\plan\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A385D758-4769-48C5-9A07-62BA263558B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E3CC61-1D72-434C-BC0D-4C30B965890D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C7E91EC6-D78D-4019-BD09-36FB01F0F196}"/>
   </bookViews>
@@ -1646,9 +1646,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>138545</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
+      <xdr:colOff>242454</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1664,7 +1664,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10424305" y="4849090"/>
-          <a:ext cx="1958195" cy="173183"/>
+          <a:ext cx="2062104" cy="190501"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1713,8 +1713,8 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1732,7 +1732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12502489" y="5039592"/>
-          <a:ext cx="1421329" cy="190499"/>
+          <a:ext cx="1559875" cy="190499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1781,10 +1781,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>138546</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1800,7 +1800,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14062364" y="5230091"/>
-          <a:ext cx="1437409" cy="173182"/>
+          <a:ext cx="1558636" cy="207818"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1844,13 +1844,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>259772</xdr:colOff>
+      <xdr:colOff>259771</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>138545</xdr:colOff>
+      <xdr:colOff>259771</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1867,8 +1867,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15620999" y="5420591"/>
-          <a:ext cx="1437410" cy="190500"/>
+          <a:off x="15620998" y="5420591"/>
+          <a:ext cx="1558637" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1917,10 +1917,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>103909</xdr:colOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1935,8 +1935,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10408227" y="2182091"/>
-          <a:ext cx="6355773" cy="190499"/>
+          <a:off x="10338954" y="2159000"/>
+          <a:ext cx="7139421" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2097,16 +2097,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>130336</xdr:colOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>146212</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>775126</xdr:rowOff>
+      <xdr:rowOff>760693</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>139861</xdr:colOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>155737</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>89326</xdr:rowOff>
+      <xdr:rowOff>74893</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2121,8 +2121,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17050200" y="1675671"/>
-          <a:ext cx="9525" cy="4977246"/>
+          <a:off x="17608712" y="1649693"/>
+          <a:ext cx="9525" cy="4965700"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2160,6 +2160,142 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rektangel 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79979860-0198-4861-8BF0-3DE30462D37A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16954500" y="5588000"/>
+          <a:ext cx="254000" cy="174625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rektangel 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4878B60-EB72-41D4-8F05-CBDAAC876804}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16954500" y="5778500"/>
+          <a:ext cx="508000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nb-NO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2464,8 +2600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522C6D6D-DA4F-4D07-9634-46F540085D48}">
   <dimension ref="A1:BP36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AR11" sqref="AR11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AP27" sqref="AP27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>